<commit_message>
Nộp đồ án Python
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -64,13 +62,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -436,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,12 +442,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,27 +466,42 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Ngày Vào</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Họ Lót</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Tên</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Giới Tính</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Ngày Sinh</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Phòng</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thành Tiền</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Trạng Thái Đóng Tiền</t>
         </is>
       </c>
     </row>
@@ -498,65 +513,47 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
+          <t>DH25PM</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
           <t>Lâm Huỳnh Phương</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Nghiêm</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Nữ</t>
         </is>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>39013</v>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>DH25PM</t>
-        </is>
-      </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
+          <t>2006-10-23</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
           <t>23</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>DPM245507</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Võ Đức</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Trọng</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>39009</v>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>DH25PM</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>19</t>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>2000000</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>Đã đóng</t>
         </is>
       </c>
     </row>

</xml_diff>